<commit_message>
Metodos Create, Update indicadores. CostosFijos bug agregar
</commit_message>
<xml_diff>
--- a/Service.Report/wwwroot/layout/excel/Indicators/IndicadoresListado.xlsx
+++ b/Service.Report/wwwroot/layout/excel/Indicators/IndicadoresListado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.Report\wwwroot\layout\excel\Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C74B92-63F3-42FD-852C-43D17337DDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7286823A-2FC1-4ED2-AA80-081E2832921A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diario" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Mensual" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Promotions" localSheetId="2">Mensual!$A$4:$E$5</definedName>
-    <definedName name="Promotions" localSheetId="1">Semanal!$A$4:$E$5</definedName>
-    <definedName name="Promotions">Diario!$A$4:$E$5</definedName>
+    <definedName name="Indicadores_Mensual" localSheetId="2">Mensual!$A$4</definedName>
+    <definedName name="Indicadores_TablaM">Mensual!$A$3:$B$5</definedName>
+    <definedName name="Sucursales_Mensual" localSheetId="2">Mensual!$B$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <r>
       <rPr>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>{{item.Sucursal}}</t>
+  </si>
+  <si>
+    <t>{{Dia}}</t>
   </si>
 </sst>
 </file>
@@ -161,10 +164,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,16 +665,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -687,7 +690,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -723,16 +726,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -748,7 +751,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -770,7 +773,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,20 +787,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -809,7 +812,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>